<commit_message>
(DONE) all NLM-LBP images are now present
</commit_message>
<xml_diff>
--- a/Python/resultados/HW_C001_120.xlsx
+++ b/Python/resultados/HW_C001_120.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="sigma_010" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="sigma_025" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="sigma_050" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,10 +464,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>27.875</v>
+        <v>27.87020078573618</v>
       </c>
       <c r="C2" t="n">
-        <v>29.234375</v>
+        <v>29.23162549921955</v>
       </c>
     </row>
     <row r="3">
@@ -474,10 +475,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>27.890625</v>
+        <v>27.89202603385473</v>
       </c>
       <c r="C3" t="n">
-        <v>29.234375</v>
+        <v>29.23162240255576</v>
       </c>
     </row>
     <row r="4">
@@ -485,10 +486,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>27.875</v>
+        <v>27.87597590032804</v>
       </c>
       <c r="C4" t="n">
-        <v>29.203125</v>
+        <v>29.20891230537436</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +497,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>27.875</v>
+        <v>27.87314307223009</v>
       </c>
       <c r="C5" t="n">
-        <v>29.21875</v>
+        <v>29.21973565966858</v>
       </c>
     </row>
     <row r="6">
@@ -507,10 +508,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>27.859375</v>
+        <v>27.85986638595025</v>
       </c>
       <c r="C6" t="n">
-        <v>29.234375</v>
+        <v>29.2356552184242</v>
       </c>
     </row>
     <row r="7">
@@ -518,10 +519,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>27.84375</v>
+        <v>27.84534987417182</v>
       </c>
       <c r="C7" t="n">
-        <v>29.234375</v>
+        <v>29.23781741192075</v>
       </c>
     </row>
     <row r="8">
@@ -529,10 +530,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>27.875</v>
+        <v>27.86789637483492</v>
       </c>
       <c r="C8" t="n">
-        <v>29.25</v>
+        <v>29.24593578672644</v>
       </c>
     </row>
     <row r="9">
@@ -540,10 +541,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>27.84375</v>
+        <v>27.84109506100912</v>
       </c>
       <c r="C9" t="n">
-        <v>29.21875</v>
+        <v>29.22349926087973</v>
       </c>
     </row>
     <row r="10">
@@ -551,10 +552,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>27.859375</v>
+        <v>27.86675187801924</v>
       </c>
       <c r="C10" t="n">
-        <v>29.25</v>
+        <v>29.24567152674653</v>
       </c>
     </row>
     <row r="11">
@@ -562,10 +563,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>27.890625</v>
+        <v>27.88841348933761</v>
       </c>
       <c r="C11" t="n">
-        <v>29.21875</v>
+        <v>29.22505043036434</v>
       </c>
     </row>
     <row r="12">
@@ -575,10 +576,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27.875</v>
+        <v>27.8680718855472</v>
       </c>
       <c r="C12" t="n">
-        <v>29.234375</v>
+        <v>29.23055255018802</v>
       </c>
     </row>
   </sheetData>
@@ -622,10 +623,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19.828125</v>
+        <v>19.83487041827138</v>
       </c>
       <c r="C2" t="n">
-        <v>26.25</v>
+        <v>26.25420099008549</v>
       </c>
     </row>
     <row r="3">
@@ -633,10 +634,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19.859375</v>
+        <v>19.85482447402956</v>
       </c>
       <c r="C3" t="n">
-        <v>26.28125</v>
+        <v>26.28165564456079</v>
       </c>
     </row>
     <row r="4">
@@ -644,10 +645,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19.828125</v>
+        <v>19.82817573284596</v>
       </c>
       <c r="C4" t="n">
-        <v>26.25</v>
+        <v>26.25192769707273</v>
       </c>
     </row>
     <row r="5">
@@ -655,10 +656,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>19.84375</v>
+        <v>19.84333235722811</v>
       </c>
       <c r="C5" t="n">
-        <v>26.25</v>
+        <v>26.25369316213408</v>
       </c>
     </row>
     <row r="6">
@@ -666,10 +667,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>19.84375</v>
+        <v>19.83980225970875</v>
       </c>
       <c r="C6" t="n">
-        <v>26.28125</v>
+        <v>26.28268614281532</v>
       </c>
     </row>
     <row r="7">
@@ -677,10 +678,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>19.828125</v>
+        <v>19.83152848847809</v>
       </c>
       <c r="C7" t="n">
-        <v>26.234375</v>
+        <v>26.23664979826602</v>
       </c>
     </row>
     <row r="8">
@@ -688,10 +689,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>19.84375</v>
+        <v>19.8364636529461</v>
       </c>
       <c r="C8" t="n">
-        <v>26.28125</v>
+        <v>26.28612151731762</v>
       </c>
     </row>
     <row r="9">
@@ -699,10 +700,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>19.828125</v>
+        <v>19.8334135560606</v>
       </c>
       <c r="C9" t="n">
-        <v>26.25</v>
+        <v>26.25514091291789</v>
       </c>
     </row>
     <row r="10">
@@ -710,10 +711,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>19.84375</v>
+        <v>19.84068486092812</v>
       </c>
       <c r="C10" t="n">
-        <v>26.265625</v>
+        <v>26.26997023483574</v>
       </c>
     </row>
     <row r="11">
@@ -721,10 +722,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19.84375</v>
+        <v>19.850774888287</v>
       </c>
       <c r="C11" t="n">
-        <v>26.265625</v>
+        <v>26.26385568623316</v>
       </c>
     </row>
     <row r="12">
@@ -734,10 +735,169 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19.84375</v>
+        <v>19.83938706887837</v>
       </c>
       <c r="C12" t="n">
-        <v>26.265625</v>
+        <v>26.26359017862389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Rows</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Noisy</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>NLM-LBP</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>14.97975563225593</v>
+      </c>
+      <c r="C2" t="n">
+        <v>21.34956152581907</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>15.0045847407783</v>
+      </c>
+      <c r="C3" t="n">
+        <v>21.41641633496312</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>14.98286819318816</v>
+      </c>
+      <c r="C4" t="n">
+        <v>21.35984420605602</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>14.98168483299892</v>
+      </c>
+      <c r="C5" t="n">
+        <v>21.34809556940976</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>14.9756225090553</v>
+      </c>
+      <c r="C6" t="n">
+        <v>21.36661623519658</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>15.00749536935757</v>
+      </c>
+      <c r="C7" t="n">
+        <v>21.26614987421846</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>14.99464126173856</v>
+      </c>
+      <c r="C8" t="n">
+        <v>21.22953702876519</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>14.98049189822739</v>
+      </c>
+      <c r="C9" t="n">
+        <v>21.29185204230119</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>14.98212362293368</v>
+      </c>
+      <c r="C10" t="n">
+        <v>21.24690564050391</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>14.99722173035512</v>
+      </c>
+      <c r="C11" t="n">
+        <v>21.27140309655436</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>14.98864897908889</v>
+      </c>
+      <c r="C12" t="n">
+        <v>21.31463815537877</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(COMPLETED) NLM-LBP resulting images
</commit_message>
<xml_diff>
--- a/Python/resultados/HW_C001_120.xlsx
+++ b/Python/resultados/HW_C001_120.xlsx
@@ -461,112 +461,112 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>27.87020078573618</v>
+        <v>27.83096748370949</v>
       </c>
       <c r="C2" t="n">
-        <v>29.23162549921955</v>
+        <v>28.84720169803776</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>27.89202603385473</v>
+        <v>27.79020060783168</v>
       </c>
       <c r="C3" t="n">
-        <v>29.23162240255576</v>
+        <v>28.81483507752534</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>27.87597590032804</v>
+        <v>27.8574254088211</v>
       </c>
       <c r="C4" t="n">
-        <v>29.20891230537436</v>
+        <v>28.84831240086282</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>27.87314307223009</v>
+        <v>27.84740778959875</v>
       </c>
       <c r="C5" t="n">
-        <v>29.21973565966858</v>
+        <v>28.88794157735925</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>27.85986638595025</v>
+        <v>27.84937074870759</v>
       </c>
       <c r="C6" t="n">
-        <v>29.2356552184242</v>
+        <v>28.85522678685512</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>27.84534987417182</v>
+        <v>27.81816264608317</v>
       </c>
       <c r="C7" t="n">
-        <v>29.23781741192075</v>
+        <v>28.84828755242988</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>27.86789637483492</v>
+        <v>27.8390060300491</v>
       </c>
       <c r="C8" t="n">
-        <v>29.24593578672644</v>
+        <v>28.84712767239659</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>27.84109506100912</v>
+        <v>27.82131605091118</v>
       </c>
       <c r="C9" t="n">
-        <v>29.22349926087973</v>
+        <v>28.84829255545864</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>27.86675187801924</v>
+        <v>27.81742838227542</v>
       </c>
       <c r="C10" t="n">
-        <v>29.24567152674653</v>
+        <v>28.83940459846023</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>27.88841348933761</v>
+        <v>27.83695446924043</v>
       </c>
       <c r="C11" t="n">
-        <v>29.22505043036434</v>
+        <v>28.83634974466139</v>
       </c>
     </row>
     <row r="12">
@@ -576,10 +576,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27.8680718855472</v>
+        <v>27.83082396172279</v>
       </c>
       <c r="C12" t="n">
-        <v>29.23055255018802</v>
+        <v>28.8472979664047</v>
       </c>
     </row>
   </sheetData>
@@ -620,112 +620,112 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>19.83487041827138</v>
+        <v>19.81360772831505</v>
       </c>
       <c r="C2" t="n">
-        <v>26.25420099008549</v>
+        <v>26.1509069501992</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>19.85482447402956</v>
+        <v>19.85848040293938</v>
       </c>
       <c r="C3" t="n">
-        <v>26.28165564456079</v>
+        <v>26.1855511587085</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>19.82817573284596</v>
+        <v>19.82127581465778</v>
       </c>
       <c r="C4" t="n">
-        <v>26.25192769707273</v>
+        <v>26.14690495315903</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>19.84333235722811</v>
+        <v>19.85354781174944</v>
       </c>
       <c r="C5" t="n">
-        <v>26.25369316213408</v>
+        <v>26.19741383258339</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>19.83980225970875</v>
+        <v>19.82843320122187</v>
       </c>
       <c r="C6" t="n">
-        <v>26.28268614281532</v>
+        <v>26.14554304271921</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>19.83152848847809</v>
+        <v>19.83117714871628</v>
       </c>
       <c r="C7" t="n">
-        <v>26.23664979826602</v>
+        <v>26.14261871513665</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>19.8364636529461</v>
+        <v>19.8267338368039</v>
       </c>
       <c r="C8" t="n">
-        <v>26.28612151731762</v>
+        <v>26.13777282359939</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>19.8334135560606</v>
+        <v>19.81918576695703</v>
       </c>
       <c r="C9" t="n">
-        <v>26.25514091291789</v>
+        <v>26.14208799493854</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>19.84068486092812</v>
+        <v>19.856709838037</v>
       </c>
       <c r="C10" t="n">
-        <v>26.26997023483574</v>
+        <v>26.21422641470159</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>19.850774888287</v>
+        <v>19.83789688697364</v>
       </c>
       <c r="C11" t="n">
-        <v>26.26385568623316</v>
+        <v>26.13966739550372</v>
       </c>
     </row>
     <row r="12">
@@ -735,10 +735,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19.83938706887837</v>
+        <v>19.83470484363714</v>
       </c>
       <c r="C12" t="n">
-        <v>26.26359017862389</v>
+        <v>26.16026932812492</v>
       </c>
     </row>
   </sheetData>
@@ -779,112 +779,112 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>14.97975563225593</v>
+        <v>14.961609172719</v>
       </c>
       <c r="C2" t="n">
-        <v>21.34956152581907</v>
+        <v>21.11189937134795</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>15.0045847407783</v>
+        <v>14.9713443928894</v>
       </c>
       <c r="C3" t="n">
-        <v>21.41641633496312</v>
+        <v>21.15951761530154</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>14.98286819318816</v>
+        <v>14.97235008889229</v>
       </c>
       <c r="C4" t="n">
-        <v>21.35984420605602</v>
+        <v>21.1558129446036</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>14.98168483299892</v>
+        <v>14.9919493135604</v>
       </c>
       <c r="C5" t="n">
-        <v>21.34809556940976</v>
+        <v>21.19527039322807</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>14.9756225090553</v>
+        <v>14.96577627950721</v>
       </c>
       <c r="C6" t="n">
-        <v>21.36661623519658</v>
+        <v>21.17988395771821</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>15.00749536935757</v>
+        <v>14.98428047187979</v>
       </c>
       <c r="C7" t="n">
-        <v>21.26614987421846</v>
+        <v>21.17596760470006</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>14.99464126173856</v>
+        <v>14.97449471337259</v>
       </c>
       <c r="C8" t="n">
-        <v>21.22953702876519</v>
+        <v>21.16236955987747</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>14.98049189822739</v>
+        <v>14.95685614272055</v>
       </c>
       <c r="C9" t="n">
-        <v>21.29185204230119</v>
+        <v>21.11077210605161</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>14.98212362293368</v>
+        <v>14.97950404299135</v>
       </c>
       <c r="C10" t="n">
-        <v>21.24690564050391</v>
+        <v>21.15126370954349</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>14.99722173035512</v>
+        <v>14.96678275407911</v>
       </c>
       <c r="C11" t="n">
-        <v>21.27140309655436</v>
+        <v>21.1296588540973</v>
       </c>
     </row>
     <row r="12">
@@ -894,10 +894,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>14.98864897908889</v>
+        <v>14.97249473726117</v>
       </c>
       <c r="C12" t="n">
-        <v>21.31463815537877</v>
+        <v>21.15324161164693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>